<commit_message>
data field excel sheet and sql queries [Documents updated]
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915E7C30-8B9E-4D44-BE83-987D4A32A46F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067129D-C1D0-4490-9E99-13020E2A0CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -72,9 +72,6 @@
     <t>Default</t>
   </si>
   <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -270,6 +267,15 @@
       </rPr>
       <t>USERHOME</t>
     </r>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -347,22 +353,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -382,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAF43974-B6DD-4163-A67B-F31BAB5ED5CF}" name="Table1" displayName="Table1" ref="G5:H9" totalsRowShown="0">
-  <autoFilter ref="G5:H9" xr:uid="{9A15A197-FC71-4B05-B5F9-4AA836C9C314}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FAF43974-B6DD-4163-A67B-F31BAB5ED5CF}" name="Table1" displayName="Table1" ref="G6:H11" totalsRowShown="0">
+  <autoFilter ref="G6:H11" xr:uid="{9A15A197-FC71-4B05-B5F9-4AA836C9C314}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1E007A80-59DE-4410-B109-1D063FC1D62A}" name="Color"/>
     <tableColumn id="2" xr3:uid="{B6562894-9B42-4C79-9872-BB78FACBE189}" name="Meaning"/>
@@ -689,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,10 +713,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -742,421 +748,443 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G8" s="6"/>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G6" s="6"/>
-      <c r="H6" t="s">
+      <c r="B9" s="11"/>
+      <c r="G9" s="2"/>
+      <c r="H9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="G7" s="2"/>
-      <c r="H7" t="s">
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>100</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B20" s="11"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="7" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="7"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29">
-        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C30">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="8" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="13"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="11"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="8"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="7"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="9">
         <v>1</v>
       </c>
-      <c r="B36" s="5" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="11"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="C45" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="9"/>
-    </row>
-    <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
+      <c r="C46" s="12"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="3" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="7"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="10"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C45:C46"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A37:B37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
completed changed to Outcome [code, data description files and database]
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9067129D-C1D0-4490-9E99-13020E2A0CA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99379656-C1B9-4350-ACC3-59534A47207A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -177,9 +177,6 @@
     <t xml:space="preserve">Description </t>
   </si>
   <si>
-    <t>completed</t>
-  </si>
-  <si>
     <t>INT (change to bool via program 0-F / 1-T)</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>outcome</t>
   </si>
 </sst>
 </file>
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -748,7 +748,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -779,15 +779,15 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -799,7 +799,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -809,7 +809,7 @@
       <c r="B9" s="11"/>
       <c r="G9" s="2"/>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -845,7 +845,7 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -919,7 +919,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>12</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>2</v>
@@ -1064,10 +1064,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
         <v>30</v>
-      </c>
-      <c r="B33" t="s">
-        <v>31</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1075,13 +1075,13 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" s="13"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="11"/>
     </row>
@@ -1093,7 +1093,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -1107,7 +1107,7 @@
     </row>
     <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>9</v>
@@ -1118,23 +1118,23 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="11"/>
     </row>
@@ -1146,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -1160,18 +1160,18 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
email made unique - Alter table
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99379656-C1B9-4350-ACC3-59534A47207A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B02AC60-8863-400B-8629-3C507B15BBC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -276,6 +277,9 @@
   </si>
   <si>
     <t>outcome</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -697,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,6 +759,9 @@
       </c>
       <c r="C4">
         <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
minor bug fixes in register and login
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F5D65C-C2B9-4531-B30C-2945EF2B1E8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C48A79-C1ED-40B4-9458-D44D0439EBD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -702,7 +701,7 @@
   <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -758,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D4" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
minor model changes and users are now added to the home with admin rights after its creation!
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C48A79-C1ED-40B4-9458-D44D0439EBD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594C7E1A-FE31-4AA0-87A0-DF9C7B0AE7AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -280,12 +280,40 @@
   <si>
     <t>UNIQUE</t>
   </si>
+  <si>
+    <r>
+      <t>Values allowed = (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u,U,a,A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>CHECK applied</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +325,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -700,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,7 +1106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>54</v>
       </c>
@@ -1082,19 +1117,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="13"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="11"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>1</v>
       </c>
@@ -1105,7 +1140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -1114,7 +1149,7 @@
       </c>
       <c r="C39" s="10"/>
     </row>
-    <row r="40" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>49</v>
       </c>
@@ -1124,8 +1159,14 @@
       <c r="C40" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1133,7 +1174,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
@@ -1141,13 +1182,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
         <v>44</v>
       </c>
       <c r="B44" s="11"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -1158,7 +1199,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>28</v>
       </c>
@@ -1167,7 +1208,7 @@
       </c>
       <c r="C46" s="12"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>47</v>
       </c>
@@ -1175,7 +1216,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
bridge table (Model) changed - details in excel + word
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594C7E1A-FE31-4AA0-87A0-DF9C7B0AE7AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6527781-C411-4999-B2BB-B9AD92EDC0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -307,6 +307,15 @@
   </si>
   <si>
     <t>CHECK applied</t>
+  </si>
+  <si>
+    <t>Home_name</t>
+  </si>
+  <si>
+    <t>varchar (60)</t>
+  </si>
+  <si>
+    <t>varchar (20)</t>
   </si>
 </sst>
 </file>
@@ -735,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1131,10 +1140,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>39</v>
@@ -1142,10 +1151,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="C39" s="10"/>
     </row>

</xml_diff>

<commit_message>
No_of_member in home functional (auto-incremented when a user is added to home)
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6527781-C411-4999-B2BB-B9AD92EDC0E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD830C2-0E92-4DB8-8A27-04AD7FCD72AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>varchar (20)</t>
+  </si>
+  <si>
+    <t>Default = 0</t>
   </si>
 </sst>
 </file>
@@ -744,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -942,7 +945,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
@@ -1112,7 +1115,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1123,7 +1126,7 @@
         <v>30</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Change in database + finding new connection string
</commit_message>
<xml_diff>
--- a/Data Fields.xlsx
+++ b/Data Fields.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saror\Desktop\Home-Sweet-Home\Home-Sweet-Home\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD830C2-0E92-4DB8-8A27-04AD7FCD72AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E88E8-D2BD-4E7E-9FE9-36373A76AF2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FD4B314-26D8-4C66-A8D1-379EE1CBD5FF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <r>
       <t xml:space="preserve">TABLE </t>
@@ -51,9 +51,6 @@
     </r>
   </si>
   <si>
-    <t>UserPk</t>
-  </si>
-  <si>
     <t>INT</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
     </r>
   </si>
   <si>
-    <t>HomePk</t>
-  </si>
-  <si>
     <t xml:space="preserve">INT </t>
   </si>
   <si>
@@ -319,6 +313,9 @@
   </si>
   <si>
     <t>Default = 0</t>
+  </si>
+  <si>
+    <t>PRIMARY KEY</t>
   </si>
 </sst>
 </file>
@@ -349,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +377,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -393,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -420,6 +423,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -747,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA0CE64-C7E3-48A4-803D-072FA42E95AA}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -769,53 +773,44 @@
       <c r="B1" s="11"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -823,27 +818,27 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>100</v>
@@ -852,75 +847,66 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G8" s="6"/>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="11"/>
       <c r="G9" s="2"/>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="G10" s="3"/>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="2">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
+      <c r="D12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>40</v>
@@ -928,10 +914,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>100</v>
@@ -939,80 +925,80 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="11"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
         <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
       </c>
       <c r="C22">
         <v>20</v>
@@ -1020,10 +1006,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>100</v>
@@ -1031,66 +1017,66 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="11"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
         <v>5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>6</v>
       </c>
       <c r="C30">
         <v>20</v>
@@ -1098,10 +1084,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>100</v>
@@ -1109,131 +1095,131 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C33" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="13"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" s="11"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="C39" s="10"/>
     </row>
     <row r="40" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="9">
         <v>1</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" s="11"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="12"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>